<commit_message>
Fixed qty of 1x2 headers
</commit_message>
<xml_diff>
--- a/communications_hub/CommBus_BOM.xlsx
+++ b/communications_hub/CommBus_BOM.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -318,10 +318,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -605,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,15 +619,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -789,11 +789,11 @@
         <v>0.2</v>
       </c>
       <c r="F8" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>1.2000000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -809,13 +809,13 @@
       <c r="D9" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>0.15</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>4</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <f t="shared" ref="G9:G20" si="1">F9*E9</f>
         <v>0.6</v>
       </c>
@@ -833,13 +833,13 @@
       <c r="D10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>0.56999999999999995</v>
       </c>
       <c r="F10" s="1">
         <v>2</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <f t="shared" si="1"/>
         <v>1.1399999999999999</v>
       </c>
@@ -857,13 +857,13 @@
       <c r="D11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>1.05</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <f t="shared" si="1"/>
         <v>1.05</v>
       </c>
@@ -881,13 +881,13 @@
       <c r="D12" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>0.94</v>
       </c>
       <c r="F12" s="1">
         <v>1</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <f t="shared" si="1"/>
         <v>0.94</v>
       </c>
@@ -905,13 +905,13 @@
       <c r="D13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>6.2</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <f t="shared" si="1"/>
         <v>6.2</v>
       </c>
@@ -929,13 +929,13 @@
       <c r="D14" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>5.15</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <f t="shared" si="1"/>
         <v>5.15</v>
       </c>
@@ -953,13 +953,13 @@
       <c r="D15" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>0.15</v>
       </c>
       <c r="F15" s="1">
         <v>4</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
@@ -983,7 +983,7 @@
       <c r="F16" s="1">
         <v>4</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <f t="shared" si="1"/>
         <v>1.8</v>
       </c>
@@ -1007,7 +1007,7 @@
       <c r="F17" s="1">
         <v>1</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <f t="shared" si="1"/>
         <v>0.46</v>
       </c>
@@ -1031,7 +1031,7 @@
       <c r="F18" s="1">
         <v>1</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
@@ -1055,7 +1055,7 @@
       <c r="F19" s="1">
         <v>1</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
@@ -1079,7 +1079,7 @@
       <c r="F20" s="1">
         <v>2</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>

</xml_diff>